<commit_message>
from M1 Macbook Air
</commit_message>
<xml_diff>
--- a/data/eval_control.xlsx
+++ b/data/eval_control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winston\workspace\PyCharm\sinewave_analyze\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainyseason/winston/Workspace/python/Pycharm Project/sinewave_analyze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80F1D13-D2E2-44D2-89E7-4D47ABFAB98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95072A9F-8C2F-B446-8116-2F60F9ED0EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="1410" windowWidth="43200" windowHeight="23475" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13420" yWindow="1420" windowWidth="43200" windowHeight="23480" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="file name" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
   <si>
     <t>filename</t>
   </si>
@@ -444,6 +444,22 @@
   </si>
   <si>
     <t>Ch2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch 4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,16 +904,16 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -932,7 +948,7 @@
         <v>300</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>125</v>
@@ -949,7 +965,7 @@
         <v>300</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>125</v>
@@ -966,7 +982,7 @@
         <v>300</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>125</v>
@@ -983,7 +999,7 @@
         <v>300</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>125</v>
@@ -1000,7 +1016,7 @@
         <v>300</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>125</v>
@@ -1017,7 +1033,7 @@
         <v>300</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>125</v>
@@ -1034,7 +1050,7 @@
         <v>300</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>125</v>
@@ -1051,7 +1067,7 @@
         <v>300</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>125</v>
@@ -1071,7 +1087,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
   </cols>
@@ -1123,7 +1139,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1159,10 +1175,10 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1198,9 +1214,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1277,13 +1293,13 @@
       <selection activeCell="E9" sqref="A2:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2024,9 +2040,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2118,10 +2134,10 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2264,11 +2280,11 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2368,10 +2384,10 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2524,10 +2540,10 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2657,11 +2673,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2759,7 +2775,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="21" style="2" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>